<commit_message>
akc rank checker done
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-1410" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,23 +12,20 @@
     <sheet name="AKC Rankings" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -39,7 +36,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,23 +59,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -423,10 +411,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -445,6 +433,13 @@
       <c r="A2" t="inlineStr">
         <is>
           <t>Food Safety Course</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>BCSS Course</t>
         </is>
       </c>
     </row>
@@ -987,7 +982,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -996,17 +991,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Search term</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Results Ranking</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
@@ -1025,7 +1020,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-11-04</t>
         </is>
       </c>
     </row>
@@ -1042,7 +1037,135 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-11-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Food Safety Course</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-11-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Food Safety Course</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2025-11-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Food Safety Course</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2025-11-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Food Safety Course</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2025-11-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Food Safety Course</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2025-11-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Food Safety Course</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-11-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Food Safety Course</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>7</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2025-11-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>BCSS Course</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2025-11-04</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added more pages to google
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -411,10 +411,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -432,12 +432,26 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Food Safety Course</t>
+          <t>Food Safety Course Level 1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
+        <is>
+          <t>Food Safety Course Level 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Food Safety Course Level 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>BCSS Course</t>
         </is>
@@ -982,7 +996,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1010,162 +1024,60 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Food Safety Course</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
+          <t>Food Safety Course Level 1</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>10</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-11-04</t>
+          <t>2025-11-06</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Food Safety Course</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
+          <t>Food Safety Course Level 2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>7</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-11-04</t>
+          <t>2025-11-06</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Food Safety Course</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
+          <t>Food Safety Course Level 3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>14</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-11-04</t>
+          <t>2025-11-06</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Food Safety Course</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
+          <t>BCSS Course</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-11-04</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Food Safety Course</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2025-11-04</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Food Safety Course</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2025-11-04</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Food Safety Course</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2025-11-04</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Food Safety Course</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>7</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2025-11-04</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Food Safety Course</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>7</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>2025-11-04</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>BCSS Course</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2025-11-04</t>
+          <t>2025-11-06</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added date time stamp
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-1410" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-1410" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -413,7 +413,7 @@
   </sheetPr>
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -881,8 +881,8 @@
   </sheetPr>
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -1028,11 +1028,11 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-11-06</t>
+          <t>2025-11-06 15:49:55</t>
         </is>
       </c>
     </row>
@@ -1043,11 +1043,11 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-11-06</t>
+          <t>2025-11-06 15:49:55</t>
         </is>
       </c>
     </row>
@@ -1058,11 +1058,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-11-06</t>
+          <t>2025-11-06 15:49:55</t>
         </is>
       </c>
     </row>
@@ -1073,11 +1073,11 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-11-06</t>
+          <t>2025-11-06 15:49:55</t>
         </is>
       </c>
     </row>

</xml_diff>